<commit_message>
- titel Feld für whiteboard tabelle; - shared tabelle erstellt
</commit_message>
<xml_diff>
--- a/db_config/sketchbook-db-draft.xlsx
+++ b/db_config/sketchbook-db-draft.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thorsten\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thorsten\Documents\Whiteboard\db_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Database</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>auto_increment</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>varchar(25)</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,28 +663,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -686,15 +686,29 @@
       <c r="C18" t="s">
         <v>9</v>
       </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>